<commit_message>
Version 2 Opti 22sec
</commit_message>
<xml_diff>
--- a/exact_duplicates.xlsx
+++ b/exact_duplicates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,6 +460,1156 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\ddn-stg-logs\sfa7k02-c1-logs.txt</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\ddn-stg-logs\ddn-stg-logs\sfa7k02-c1-logs.txt</t>
+        </is>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>sfa7k02-c1-logs.txt</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>sfa7k02-c1-logs.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\ddn-stg-logs\sfa7k02-co-logs.txt</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\ddn-stg-logs\ddn-stg-logs\sfa7k02-co-logs.txt</t>
+        </is>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>sfa7k02-co-logs.txt</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>sfa7k02-co-logs.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio1.sh</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio-bm\fio1.sh</t>
+        </is>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>fio1.sh</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>fio1.sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio10.sh</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio-bm\fio10.sh</t>
+        </is>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>fio10.sh</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>fio10.sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio22.sh</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio-bm\fio22.sh</t>
+        </is>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>fio22.sh</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>fio22.sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio-bm\fio</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio-bm\flash\fio</t>
+        </is>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>fio</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>fio</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
+        </is>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>.DS_Store</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>.DS_Store</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
+        </is>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>.DS_Store</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>.DS_Store</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
+        </is>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>.DS_Store</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>.DS_Store</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
+        </is>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>.DS_Store</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>.DS_Store</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\08456059.pdf</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\08456059.pdf</t>
+        </is>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>08456059.pdf</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>08456059.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\20180006549.pdf</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\20180006549.pdf</t>
+        </is>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>20180006549.pdf</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>20180006549.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\235434231_RAW_PAN.pix</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\235434231_RAW_PAN.pix</t>
+        </is>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>235434231_RAW_PAN.pix</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>235434231_RAW_PAN.pix</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\235434251_RAW_PAN_LOG.txt</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\235434251_RAW_PAN_LOG.txt</t>
+        </is>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>235434251_RAW_PAN_LOG.txt</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>235434251_RAW_PAN_LOG.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\3.205-CVE_to_be_installed.txt</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\3.205-CVE_to_be_installed.txt</t>
+        </is>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>3.205-CVE_to_be_installed.txt</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>3.205-CVE_to_be_installed.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\3.207-CVE_to_be_installed.txt</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\3.207-CVE_to_be_installed.txt</t>
+        </is>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>3.207-CVE_to_be_installed.txt</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>3.207-CVE_to_be_installed.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\anaconda-ks.cfg</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\anaconda-ks.cfg</t>
+        </is>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>anaconda-ks.cfg</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>anaconda-ks.cfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\authorized_keys-4-8-17</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\authorized_keys-4-8-17</t>
+        </is>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>authorized_keys-4-8-17</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>authorized_keys-4-8-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\BAND_RPC.txt</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\BAND_RPC.txt</t>
+        </is>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>BAND_RPC.txt</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>BAND_RPC.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\buttons.print.min.js</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\buttons.print.min.js</t>
+        </is>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>buttons.print.min.js</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>buttons.print.min.js</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\catalina.2023-07-14.log</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\catalina.2023-07-14.log</t>
+        </is>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>catalina.2023-07-14.log</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>catalina.2023-07-14.log</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\catalina.2023-07-16.log</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\catalina.2023-07-16.log</t>
+        </is>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>catalina.2023-07-16.log</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>catalina.2023-07-16.log</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\catalina.2023-07-23.log</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\catalina.2023-07-23.log</t>
+        </is>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>catalina.2023-07-23.log</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>catalina.2023-07-23.log</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\catalina.2023-08-26.log</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\catalina.2023-08-26.log</t>
+        </is>
+      </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>catalina.2023-08-26.log</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>catalina.2023-08-26.log</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\covid_excel_20-38.xlsx</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\covid_excel_20-38.xlsx</t>
+        </is>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>covid_excel_20-38.xlsx</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>covid_excel_20-38.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
+        </is>
+      </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
+        </is>
+      </c>
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\fio-3.1-1.el6.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\fio-3.1-1.el6.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>fio-3.1-1.el6.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>fio-3.1-1.el6.x86_64.rpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\gwm66c08.jpg</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gwm66c08.jpg</t>
+        </is>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>gwm66c08.jpg</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>gwm66c08.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\import CSV.txt</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\import CSV.txt</t>
+        </is>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>import CSV.txt</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>import CSV.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\KKD geo tagging (1).xlsx</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\KKD geo tagging (1).xlsx</t>
+        </is>
+      </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>KKD geo tagging (1).xlsx</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>KKD geo tagging (1).xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\LS____.pdf</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\LS____.pdf</t>
+        </is>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>LS____.pdf</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>LS____.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\mmhealth.sh</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\mmhealth.sh</t>
+        </is>
+      </c>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>mmhealth.sh</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>mmhealth.sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\mounted</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\mounted</t>
+        </is>
+      </c>
+      <c r="C36" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>mounted</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>mounted</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\NewGCPs.bk</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\NewGCPs.bk</t>
+        </is>
+      </c>
+      <c r="C37" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>NewGCPs.bk</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>NewGCPs.bk</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
+        </is>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
+        </is>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\syslog</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\syslog</t>
+        </is>
+      </c>
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>syslog</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>syslog</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\table.sql</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\table.sql</t>
+        </is>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>table.sql</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>table.sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.base-4.2.3-0.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\client-rpms-upgrade-withgpl\client-rpms-upgrade\gpfs.base-4.2.3-0.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>gpfs.base-4.2.3-0.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>gpfs.base-4.2.3-0.x86_64.rpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.docs-4.2.3-0.noarch.rpm</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\client-rpms-upgrade-withgpl\client-rpms-upgrade\gpfs.docs-4.2.3-0.noarch.rpm</t>
+        </is>
+      </c>
+      <c r="C43" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>gpfs.docs-4.2.3-0.noarch.rpm</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>gpfs.docs-4.2.3-0.noarch.rpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.ext-4.2.3-0.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\client-rpms-upgrade-withgpl\client-rpms-upgrade\gpfs.ext-4.2.3-0.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="C44" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>gpfs.ext-4.2.3-0.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>gpfs.ext-4.2.3-0.x86_64.rpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.gpl-4.2.3-0.noarch.rpm</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\client-rpms-upgrade-withgpl\client-rpms-upgrade\gpfs.gpl-4.2.3-0.noarch.rpm</t>
+        </is>
+      </c>
+      <c r="C45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>gpfs.gpl-4.2.3-0.noarch.rpm</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>gpfs.gpl-4.2.3-0.noarch.rpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.gplbin-3.10.0-327.el7.x86_64-4.2.3-0.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\client-rpms-upgrade-withgpl\client-rpms-upgrade\gpfs.gplbin-3.10.0-327.el7.x86_64-4.2.3-0.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="C46" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>gpfs.gplbin-3.10.0-327.el7.x86_64-4.2.3-0.x86_64.rpm</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>gpfs.gplbin-3.10.0-327.el7.x86_64-4.2.3-0.x86_64.rpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.msg.en_US-4.2.3-0.noarch.rpm</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\client-rpms-upgrade-withgpl\client-rpms-upgrade\gpfs.msg.en_US-4.2.3-0.noarch.rpm</t>
+        </is>
+      </c>
+      <c r="C47" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>gpfs.msg.en_US-4.2.3-0.noarch.rpm</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>gpfs.msg.en_US-4.2.3-0.noarch.rpm</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Version 2.2 20 sec
</commit_message>
<xml_diff>
--- a/exact_duplicates.xlsx
+++ b/exact_duplicates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,112 +463,112 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\ddn-stg-logs\sfa7k02-c1-logs.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\ddn-stg-logs\ddn-stg-logs\sfa7k02-c1-logs.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
         </is>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sfa7k02-c1-logs.txt</t>
+          <t>.DS_Store</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>sfa7k02-c1-logs.txt</t>
+          <t>.DS_Store</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\ddn-stg-logs\sfa7k02-co-logs.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\ddn-stg-logs\ddn-stg-logs\sfa7k02-co-logs.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
         </is>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sfa7k02-co-logs.txt</t>
+          <t>.DS_Store</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>sfa7k02-co-logs.txt</t>
+          <t>.DS_Store</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio1.sh</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio-bm\fio1.sh</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
         </is>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>fio1.sh</t>
+          <t>.DS_Store</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>fio1.sh</t>
+          <t>.DS_Store</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio10.sh</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio-bm\fio10.sh</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
         </is>
       </c>
       <c r="C5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>fio10.sh</t>
+          <t>.DS_Store</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>fio10.sh</t>
+          <t>.DS_Store</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio22.sh</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\08456059.pdf</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio-bm\fio22.sh</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\08456059.pdf</t>
         </is>
       </c>
       <c r="C6" t="b">
@@ -576,24 +576,24 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>fio22.sh</t>
+          <t>08456059.pdf</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>fio22.sh</t>
+          <t>08456059.pdf</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio-bm\fio</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\20180006549.pdf</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\fio-bm\fio-bm\flash\fio</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\20180006549.pdf</t>
         </is>
       </c>
       <c r="C7" t="b">
@@ -601,124 +601,124 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>fio</t>
+          <t>20180006549.pdf</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>fio</t>
+          <t>20180006549.pdf</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\235434231_RAW_PAN.pix</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\235434231_RAW_PAN.pix</t>
         </is>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>.DS_Store</t>
+          <t>235434231_RAW_PAN.pix</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>.DS_Store</t>
+          <t>235434231_RAW_PAN.pix</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\235434251_RAW_PAN_LOG.txt</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\235434251_RAW_PAN_LOG.txt</t>
         </is>
       </c>
       <c r="C9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>.DS_Store</t>
+          <t>235434251_RAW_PAN_LOG.txt</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>.DS_Store</t>
+          <t>235434251_RAW_PAN_LOG.txt</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\3.205-CVE_to_be_installed.txt</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\3.205-CVE_to_be_installed.txt</t>
         </is>
       </c>
       <c r="C10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>.DS_Store</t>
+          <t>3.205-CVE_to_be_installed.txt</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>.DS_Store</t>
+          <t>3.205-CVE_to_be_installed.txt</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\3.207-CVE_to_be_installed.txt</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\3.207-CVE_to_be_installed.txt</t>
         </is>
       </c>
       <c r="C11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>.DS_Store</t>
+          <t>3.207-CVE_to_be_installed.txt</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>.DS_Store</t>
+          <t>3.207-CVE_to_be_installed.txt</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\08456059.pdf</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\anaconda-ks.cfg</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\08456059.pdf</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\anaconda-ks.cfg</t>
         </is>
       </c>
       <c r="C12" t="b">
@@ -726,24 +726,24 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>08456059.pdf</t>
+          <t>anaconda-ks.cfg</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>08456059.pdf</t>
+          <t>anaconda-ks.cfg</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\20180006549.pdf</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\authorized_keys-4-8-17</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\20180006549.pdf</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\authorized_keys-4-8-17</t>
         </is>
       </c>
       <c r="C13" t="b">
@@ -751,24 +751,24 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>20180006549.pdf</t>
+          <t>authorized_keys-4-8-17</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>20180006549.pdf</t>
+          <t>authorized_keys-4-8-17</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\235434231_RAW_PAN.pix</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\BAND_RPC.txt</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\235434231_RAW_PAN.pix</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\BAND_RPC.txt</t>
         </is>
       </c>
       <c r="C14" t="b">
@@ -776,24 +776,24 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>235434231_RAW_PAN.pix</t>
+          <t>BAND_RPC.txt</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>235434231_RAW_PAN.pix</t>
+          <t>BAND_RPC.txt</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\235434251_RAW_PAN_LOG.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\buttons.print.min.js</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\235434251_RAW_PAN_LOG.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\buttons.print.min.js</t>
         </is>
       </c>
       <c r="C15" t="b">
@@ -801,24 +801,24 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>235434251_RAW_PAN_LOG.txt</t>
+          <t>buttons.print.min.js</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>235434251_RAW_PAN_LOG.txt</t>
+          <t>buttons.print.min.js</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\3.205-CVE_to_be_installed.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\catalina.2023-07-14.log</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\3.205-CVE_to_be_installed.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\catalina.2023-07-14.log</t>
         </is>
       </c>
       <c r="C16" t="b">
@@ -826,24 +826,24 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3.205-CVE_to_be_installed.txt</t>
+          <t>catalina.2023-07-14.log</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3.205-CVE_to_be_installed.txt</t>
+          <t>catalina.2023-07-14.log</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\3.207-CVE_to_be_installed.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\catalina.2023-07-16.log</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\3.207-CVE_to_be_installed.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\catalina.2023-07-16.log</t>
         </is>
       </c>
       <c r="C17" t="b">
@@ -851,24 +851,24 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>3.207-CVE_to_be_installed.txt</t>
+          <t>catalina.2023-07-16.log</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>3.207-CVE_to_be_installed.txt</t>
+          <t>catalina.2023-07-16.log</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\anaconda-ks.cfg</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\catalina.2023-07-23.log</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\anaconda-ks.cfg</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\catalina.2023-07-23.log</t>
         </is>
       </c>
       <c r="C18" t="b">
@@ -876,24 +876,24 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>anaconda-ks.cfg</t>
+          <t>catalina.2023-07-23.log</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>anaconda-ks.cfg</t>
+          <t>catalina.2023-07-23.log</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\authorized_keys-4-8-17</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\catalina.2023-08-26.log</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\authorized_keys-4-8-17</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\catalina.2023-08-26.log</t>
         </is>
       </c>
       <c r="C19" t="b">
@@ -901,24 +901,24 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>authorized_keys-4-8-17</t>
+          <t>catalina.2023-08-26.log</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>authorized_keys-4-8-17</t>
+          <t>catalina.2023-08-26.log</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\BAND_RPC.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\covid_excel_20-38.xlsx</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\BAND_RPC.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\covid_excel_20-38.xlsx</t>
         </is>
       </c>
       <c r="C20" t="b">
@@ -926,24 +926,24 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>BAND_RPC.txt</t>
+          <t>covid_excel_20-38.xlsx</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>BAND_RPC.txt</t>
+          <t>covid_excel_20-38.xlsx</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\buttons.print.min.js</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\buttons.print.min.js</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
         </is>
       </c>
       <c r="C21" t="b">
@@ -951,24 +951,24 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>buttons.print.min.js</t>
+          <t>ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>buttons.print.min.js</t>
+          <t>ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\catalina.2023-07-14.log</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\catalina.2023-07-14.log</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
         </is>
       </c>
       <c r="C22" t="b">
@@ -976,24 +976,24 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>catalina.2023-07-14.log</t>
+          <t>EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>catalina.2023-07-14.log</t>
+          <t>EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\catalina.2023-07-16.log</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\fio-3.1-1.el6.x86_64.rpm</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\catalina.2023-07-16.log</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\fio-3.1-1.el6.x86_64.rpm</t>
         </is>
       </c>
       <c r="C23" t="b">
@@ -1001,24 +1001,24 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>catalina.2023-07-16.log</t>
+          <t>fio-3.1-1.el6.x86_64.rpm</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>catalina.2023-07-16.log</t>
+          <t>fio-3.1-1.el6.x86_64.rpm</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\catalina.2023-07-23.log</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\catalina.2023-07-23.log</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
         </is>
       </c>
       <c r="C24" t="b">
@@ -1026,24 +1026,24 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>catalina.2023-07-23.log</t>
+          <t>gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>catalina.2023-07-23.log</t>
+          <t>gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\catalina.2023-08-26.log</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\gwm66c08.jpg</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\catalina.2023-08-26.log</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\gwm66c08.jpg</t>
         </is>
       </c>
       <c r="C25" t="b">
@@ -1051,24 +1051,24 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>catalina.2023-08-26.log</t>
+          <t>gwm66c08.jpg</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>catalina.2023-08-26.log</t>
+          <t>gwm66c08.jpg</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\covid_excel_20-38.xlsx</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\import CSV.txt</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\covid_excel_20-38.xlsx</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\import CSV.txt</t>
         </is>
       </c>
       <c r="C26" t="b">
@@ -1076,24 +1076,24 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>covid_excel_20-38.xlsx</t>
+          <t>import CSV.txt</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>covid_excel_20-38.xlsx</t>
+          <t>import CSV.txt</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\KKD geo tagging (1).xlsx</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\KKD geo tagging (1).xlsx</t>
         </is>
       </c>
       <c r="C27" t="b">
@@ -1101,24 +1101,24 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
+          <t>KKD geo tagging (1).xlsx</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
+          <t>KKD geo tagging (1).xlsx</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\LS____.pdf</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\LS____.pdf</t>
         </is>
       </c>
       <c r="C28" t="b">
@@ -1126,24 +1126,24 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
+          <t>LS____.pdf</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
+          <t>LS____.pdf</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\fio-3.1-1.el6.x86_64.rpm</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\mmhealth.sh</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\fio-3.1-1.el6.x86_64.rpm</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\mmhealth.sh</t>
         </is>
       </c>
       <c r="C29" t="b">
@@ -1151,24 +1151,24 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>fio-3.1-1.el6.x86_64.rpm</t>
+          <t>mmhealth.sh</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>fio-3.1-1.el6.x86_64.rpm</t>
+          <t>mmhealth.sh</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\mounted</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\mounted</t>
         </is>
       </c>
       <c r="C30" t="b">
@@ -1176,24 +1176,24 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
+          <t>mounted</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
+          <t>mounted</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\gwm66c08.jpg</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\NewGCPs.bk</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gwm66c08.jpg</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\NewGCPs.bk</t>
         </is>
       </c>
       <c r="C31" t="b">
@@ -1201,24 +1201,24 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>gwm66c08.jpg</t>
+          <t>NewGCPs.bk</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>gwm66c08.jpg</t>
+          <t>NewGCPs.bk</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\import CSV.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\import CSV.txt</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
         </is>
       </c>
       <c r="C32" t="b">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>import CSV.txt</t>
+          <t>SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>import CSV.txt</t>
+          <t>SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\KKD geo tagging (1).xlsx</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\KKD geo tagging (1).xlsx</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
         </is>
       </c>
       <c r="C33" t="b">
@@ -1251,24 +1251,24 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>KKD geo tagging (1).xlsx</t>
+          <t>SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>KKD geo tagging (1).xlsx</t>
+          <t>SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\LS____.pdf</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\syslog</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\LS____.pdf</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\syslog</t>
         </is>
       </c>
       <c r="C34" t="b">
@@ -1276,24 +1276,24 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>LS____.pdf</t>
+          <t>syslog</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>LS____.pdf</t>
+          <t>syslog</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\mmhealth.sh</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\table.sql</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\mmhealth.sh</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\table.sql</t>
         </is>
       </c>
       <c r="C35" t="b">
@@ -1301,312 +1301,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>mmhealth.sh</t>
+          <t>table.sql</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>mmhealth.sh</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\mounted</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\mounted</t>
-        </is>
-      </c>
-      <c r="C36" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>mounted</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>mounted</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\NewGCPs.bk</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\NewGCPs.bk</t>
-        </is>
-      </c>
-      <c r="C37" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>NewGCPs.bk</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>NewGCPs.bk</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
-        </is>
-      </c>
-      <c r="C38" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
-        </is>
-      </c>
-      <c r="C39" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\syslog</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\syslog</t>
-        </is>
-      </c>
-      <c r="C40" t="b">
-        <v>1</v>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>syslog</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>syslog</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-1\table.sql</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\table.sql</t>
-        </is>
-      </c>
-      <c r="C41" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
           <t>table.sql</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>table.sql</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.base-4.2.3-0.x86_64.rpm</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\client-rpms-upgrade-withgpl\client-rpms-upgrade\gpfs.base-4.2.3-0.x86_64.rpm</t>
-        </is>
-      </c>
-      <c r="C42" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>gpfs.base-4.2.3-0.x86_64.rpm</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>gpfs.base-4.2.3-0.x86_64.rpm</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.docs-4.2.3-0.noarch.rpm</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\client-rpms-upgrade-withgpl\client-rpms-upgrade\gpfs.docs-4.2.3-0.noarch.rpm</t>
-        </is>
-      </c>
-      <c r="C43" t="b">
-        <v>1</v>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>gpfs.docs-4.2.3-0.noarch.rpm</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>gpfs.docs-4.2.3-0.noarch.rpm</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.ext-4.2.3-0.x86_64.rpm</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\client-rpms-upgrade-withgpl\client-rpms-upgrade\gpfs.ext-4.2.3-0.x86_64.rpm</t>
-        </is>
-      </c>
-      <c r="C44" t="b">
-        <v>1</v>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>gpfs.ext-4.2.3-0.x86_64.rpm</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>gpfs.ext-4.2.3-0.x86_64.rpm</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.gpl-4.2.3-0.noarch.rpm</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\client-rpms-upgrade-withgpl\client-rpms-upgrade\gpfs.gpl-4.2.3-0.noarch.rpm</t>
-        </is>
-      </c>
-      <c r="C45" t="b">
-        <v>1</v>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>gpfs.gpl-4.2.3-0.noarch.rpm</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>gpfs.gpl-4.2.3-0.noarch.rpm</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.gplbin-3.10.0-327.el7.x86_64-4.2.3-0.x86_64.rpm</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\client-rpms-upgrade-withgpl\client-rpms-upgrade\gpfs.gplbin-3.10.0-327.el7.x86_64-4.2.3-0.x86_64.rpm</t>
-        </is>
-      </c>
-      <c r="C46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>gpfs.gplbin-3.10.0-327.el7.x86_64-4.2.3-0.x86_64.rpm</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>gpfs.gplbin-3.10.0-327.el7.x86_64-4.2.3-0.x86_64.rpm</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\gpfs.msg.en_US-4.2.3-0.noarch.rpm</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\Data RR\\dataset1\folder-2\client-rpms-upgrade-withgpl\client-rpms-upgrade\gpfs.msg.en_US-4.2.3-0.noarch.rpm</t>
-        </is>
-      </c>
-      <c r="C47" t="b">
-        <v>1</v>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>gpfs.msg.en_US-4.2.3-0.noarch.rpm</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>gpfs.msg.en_US-4.2.3-0.noarch.rpm</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Version 3 With graph
</commit_message>
<xml_diff>
--- a/exact_duplicates.xlsx
+++ b/exact_duplicates.xlsx
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
         </is>
       </c>
       <c r="C2" t="b">
@@ -488,12 +488,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
         </is>
       </c>
       <c r="C3" t="b">
@@ -513,12 +513,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
         </is>
       </c>
       <c r="C4" t="b">
@@ -538,12 +538,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\aa\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
+          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
         </is>
       </c>
       <c r="C5" t="b">

</xml_diff>

<commit_message>
Version 5 Created picture dataset for siamese
</commit_message>
<xml_diff>
--- a/exact_duplicates.xlsx
+++ b/exact_duplicates.xlsx
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
         </is>
       </c>
       <c r="C2" t="b">
@@ -488,12 +488,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
         </is>
       </c>
       <c r="C3" t="b">
@@ -513,12 +513,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
         </is>
       </c>
       <c r="C4" t="b">
@@ -538,12 +538,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\.DS_Store</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\Docs\.DS_Store</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\.tar\opt\ddn\others\RAW_BM\XDD\xdd_r4563_20150503\xdd\bin\.DS_Store</t>
         </is>
       </c>
       <c r="C5" t="b">
@@ -563,12 +563,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\08456059.pdf</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\08456059.pdf</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\08456059.pdf</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\08456059.pdf</t>
         </is>
       </c>
       <c r="C6" t="b">
@@ -588,12 +588,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\20180006549.pdf</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\20180006549.pdf</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\20180006549.pdf</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\20180006549.pdf</t>
         </is>
       </c>
       <c r="C7" t="b">
@@ -613,12 +613,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\235434231_RAW_PAN.pix</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\235434231_RAW_PAN.pix</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\235434231_RAW_PAN.pix</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\235434231_RAW_PAN.pix</t>
         </is>
       </c>
       <c r="C8" t="b">
@@ -638,12 +638,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\235434251_RAW_PAN_LOG.txt</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\235434251_RAW_PAN_LOG.txt</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\235434251_RAW_PAN_LOG.txt</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\235434251_RAW_PAN_LOG.txt</t>
         </is>
       </c>
       <c r="C9" t="b">
@@ -663,12 +663,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\3.205-CVE_to_be_installed.txt</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\3.205-CVE_to_be_installed.txt</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\3.205-CVE_to_be_installed.txt</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\3.205-CVE_to_be_installed.txt</t>
         </is>
       </c>
       <c r="C10" t="b">
@@ -688,12 +688,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\3.207-CVE_to_be_installed.txt</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\3.207-CVE_to_be_installed.txt</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\3.207-CVE_to_be_installed.txt</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\3.207-CVE_to_be_installed.txt</t>
         </is>
       </c>
       <c r="C11" t="b">
@@ -713,12 +713,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\anaconda-ks.cfg</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\anaconda-ks.cfg</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\anaconda-ks.cfg</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\anaconda-ks.cfg</t>
         </is>
       </c>
       <c r="C12" t="b">
@@ -738,12 +738,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\authorized_keys-4-8-17</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\authorized_keys-4-8-17</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\authorized_keys-4-8-17</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\authorized_keys-4-8-17</t>
         </is>
       </c>
       <c r="C13" t="b">
@@ -763,12 +763,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\BAND_RPC.txt</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\BAND_RPC.txt</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\BAND_RPC.txt</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\BAND_RPC.txt</t>
         </is>
       </c>
       <c r="C14" t="b">
@@ -788,12 +788,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\buttons.print.min.js</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\buttons.print.min.js</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\buttons.print.min.js</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\buttons.print.min.js</t>
         </is>
       </c>
       <c r="C15" t="b">
@@ -813,12 +813,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\catalina.2023-07-14.log</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\catalina.2023-07-14.log</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\catalina.2023-07-14.log</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\catalina.2023-07-14.log</t>
         </is>
       </c>
       <c r="C16" t="b">
@@ -838,12 +838,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\catalina.2023-07-16.log</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\catalina.2023-07-16.log</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\catalina.2023-07-16.log</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\catalina.2023-07-16.log</t>
         </is>
       </c>
       <c r="C17" t="b">
@@ -863,12 +863,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\catalina.2023-07-23.log</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\catalina.2023-07-23.log</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\catalina.2023-07-23.log</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\catalina.2023-07-23.log</t>
         </is>
       </c>
       <c r="C18" t="b">
@@ -888,12 +888,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\catalina.2023-08-26.log</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\catalina.2023-08-26.log</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\catalina.2023-08-26.log</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\catalina.2023-08-26.log</t>
         </is>
       </c>
       <c r="C19" t="b">
@@ -913,12 +913,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\covid_excel_20-38.xlsx</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\covid_excel_20-38.xlsx</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\covid_excel_20-38.xlsx</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\covid_excel_20-38.xlsx</t>
         </is>
       </c>
       <c r="C20" t="b">
@@ -938,12 +938,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\ddn-restapi-core-gs-4.2.1-3.3d53e4_dirty.noarch.rpm</t>
         </is>
       </c>
       <c r="C21" t="b">
@@ -963,12 +963,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\EaseUS Partition Master 9.2.2 Technician Edition (FULL + Patch).zip</t>
         </is>
       </c>
       <c r="C22" t="b">
@@ -988,12 +988,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\fio-3.1-1.el6.x86_64.rpm</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\fio-3.1-1.el6.x86_64.rpm</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\fio-3.1-1.el6.x86_64.rpm</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\fio-3.1-1.el6.x86_64.rpm</t>
         </is>
       </c>
       <c r="C23" t="b">
@@ -1013,12 +1013,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\gpfs.gss.pmsensors-4.2.3-5.el7.x86_64.rpm</t>
         </is>
       </c>
       <c r="C24" t="b">
@@ -1038,12 +1038,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\gwm66c08.jpg</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\gwm66c08.jpg</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\gwm66c08.jpg</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\gwm66c08.jpg</t>
         </is>
       </c>
       <c r="C25" t="b">
@@ -1063,12 +1063,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\import CSV.txt</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\import CSV.txt</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\import CSV.txt</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\import CSV.txt</t>
         </is>
       </c>
       <c r="C26" t="b">
@@ -1088,12 +1088,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\KKD geo tagging (1).xlsx</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\KKD geo tagging (1).xlsx</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\KKD geo tagging (1).xlsx</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\KKD geo tagging (1).xlsx</t>
         </is>
       </c>
       <c r="C27" t="b">
@@ -1113,12 +1113,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\LS____.pdf</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\LS____.pdf</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\LS____.pdf</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\LS____.pdf</t>
         </is>
       </c>
       <c r="C28" t="b">
@@ -1138,12 +1138,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\mmhealth.sh</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\mmhealth.sh</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\mmhealth.sh</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\mmhealth.sh</t>
         </is>
       </c>
       <c r="C29" t="b">
@@ -1163,12 +1163,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\mounted</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\mounted</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\mounted</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\mounted</t>
         </is>
       </c>
       <c r="C30" t="b">
@@ -1188,12 +1188,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\NewGCPs.bk</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\NewGCPs.bk</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\NewGCPs.bk</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\NewGCPs.bk</t>
         </is>
       </c>
       <c r="C31" t="b">
@@ -1213,12 +1213,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\SR159360_ddn_showall_20210222-13_54_51.tar.gz</t>
         </is>
       </c>
       <c r="C32" t="b">
@@ -1238,12 +1238,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\SR170158_ddn_showall_20210902-13_20_38.tar.gz</t>
         </is>
       </c>
       <c r="C33" t="b">
@@ -1263,12 +1263,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\syslog</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\syslog</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\syslog</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\syslog</t>
         </is>
       </c>
       <c r="C34" t="b">
@@ -1288,12 +1288,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-1\table.sql</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-1\table.sql</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>D:\\adhvik\\adh\\Hackathon\\space hack\\top12 data\\topic12\\dataset1\folder-2\table.sql</t>
+          <t>D:\adhvik\adh\Hackathon\space hack\Data RR\data Set\topic12\dataset1\folder-2\table.sql</t>
         </is>
       </c>
       <c r="C35" t="b">

</xml_diff>